<commit_message>
Fixed the blank year_ending case and PR comments
</commit_message>
<xml_diff>
--- a/seed/tests/data/Sample_MultipleCycles.xlsx
+++ b/seed/tests/data/Sample_MultipleCycles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achapin/seed/seed/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090C996B-729F-0849-8F94-E3264CBEC32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD2C5D0-0F53-2140-A3CF-A351C4733924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="7780" windowWidth="38400" windowHeight="19860" xr2:uid="{15E2FF8E-BDE4-2645-8996-E71827398BCF}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19860" xr2:uid="{15E2FF8E-BDE4-2645-8996-E71827398BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="27">
   <si>
     <t>Property Id</t>
   </si>
@@ -575,13 +575,13 @@
   <sheetPr codeName="Sheet11">
     <tabColor theme="7" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -657,7 +657,7 @@
         <v>26</v>
       </c>
       <c r="C2" s="5">
-        <v>44196</v>
+        <v>44197</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>19</v>
@@ -716,7 +716,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="5">
-        <v>43830</v>
+        <v>44196</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>19</v>
@@ -740,10 +740,10 @@
         <v>23</v>
       </c>
       <c r="K3" s="6">
-        <v>228.9</v>
+        <v>207.1</v>
       </c>
       <c r="L3" s="6">
-        <v>228.9</v>
+        <v>207.1</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>23</v>
@@ -758,13 +758,13 @@
         <v>24</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="R3" s="6">
-        <v>701500.6</v>
+        <v>630245.30000000005</v>
       </c>
       <c r="S3" s="6">
-        <v>1829118.4</v>
+        <v>1655183.7</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -775,7 +775,7 @@
         <v>26</v>
       </c>
       <c r="C4" s="5">
-        <v>43465</v>
+        <v>43830</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>19</v>
@@ -799,30 +799,146 @@
         <v>23</v>
       </c>
       <c r="K4" s="6">
+        <v>228.9</v>
+      </c>
+      <c r="L4" s="6">
+        <v>228.9</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R4" s="6">
+        <v>701500.6</v>
+      </c>
+      <c r="S4" s="6">
+        <v>1829118.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>2045373</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="5">
+        <v>43465</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="6">
+        <v>7992</v>
+      </c>
+      <c r="I5" s="6">
+        <v>7992</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="6">
         <v>238.4</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L5" s="6">
         <v>238.4</v>
       </c>
-      <c r="M4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="R4" s="6">
+      <c r="M5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R5" s="6">
         <v>724279.4</v>
       </c>
-      <c r="S4" s="6">
+      <c r="S5" s="6">
+        <v>1905372.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>2045374</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="6">
+        <v>7992</v>
+      </c>
+      <c r="I6" s="6">
+        <v>7992</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="6">
+        <v>238.4</v>
+      </c>
+      <c r="L6" s="6">
+        <v>238.4</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R6" s="6">
+        <v>724279.4</v>
+      </c>
+      <c r="S6" s="6">
         <v>1905372.9</v>
       </c>
     </row>

</xml_diff>